<commit_message>
Add configuration GUI with config.ini, Add abillity to add more collumns
</commit_message>
<xml_diff>
--- a/route-planner/template.xlsx
+++ b/route-planner/template.xlsx
@@ -5,15 +5,17 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dor\PycharmProjects\route-planner\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Dor\Desktop\technion\caring-heart\route-planner\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2B1EE643-486C-4ACC-9075-13A28F6FC74D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6196F4FA-BF95-44CE-A76C-5CD4889AE123}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="גיליון1" sheetId="1" r:id="rId1"/>
+    <sheet name="Sheet1" sheetId="2" r:id="rId2"/>
+    <sheet name="Sheet2" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="0"/>
 </workbook>
@@ -519,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J100"/>
+  <dimension ref="A1:K100"/>
   <sheetViews>
     <sheetView rightToLeft="1" tabSelected="1" workbookViewId="0">
-      <selection activeCell="H16" sqref="H16"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="14.3984375" defaultRowHeight="15" customHeight="1" x14ac:dyDescent="0.25"/>
@@ -534,7 +536,7 @@
     <col min="10" max="11" width="8.69921875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.3">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -566,69 +568,84 @@
         <v>9</v>
       </c>
     </row>
-    <row r="2" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I2" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B3" t="s">
         <v>25</v>
       </c>
       <c r="I3" s="7"/>
-    </row>
-    <row r="4" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K3">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B4" t="s">
         <v>23</v>
       </c>
       <c r="I4" s="7"/>
-    </row>
-    <row r="5" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K4">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B5" t="s">
         <v>24</v>
       </c>
       <c r="I5" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="6" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K5">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="B6" t="s">
         <v>26</v>
       </c>
       <c r="I6" s="7"/>
-    </row>
-    <row r="7" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="K6">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I7" s="7"/>
     </row>
-    <row r="8" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I8" s="7"/>
     </row>
-    <row r="9" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I9" s="7"/>
     </row>
-    <row r="10" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I10" s="8"/>
     </row>
-    <row r="11" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I11" s="8"/>
     </row>
-    <row r="12" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I12" s="6" t="s">
         <v>10</v>
       </c>
     </row>
-    <row r="13" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I13" s="9" t="s">
         <v>12</v>
       </c>
     </row>
-    <row r="14" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I14" s="7"/>
     </row>
-    <row r="15" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I15" s="7"/>
     </row>
-    <row r="16" spans="1:10" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:11" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
       <c r="I16" s="7"/>
     </row>
     <row r="17" spans="9:9" ht="14.25" customHeight="1" x14ac:dyDescent="0.25">
@@ -895,4 +912,30 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0" footer="0"/>
   <pageSetup orientation="landscape"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{079C6879-34D6-45D9-8C4D-620A71475E02}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D977569E-05EE-4741-AD5B-5886A9225ED1}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="D30" sqref="D30"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>